<commit_message>
Replace photo.jpg with photo.png and update resume.xlsx
</commit_message>
<xml_diff>
--- a/resume.xlsx
+++ b/resume.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Resume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F1C888-36A6-4614-A60D-314CB7424BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674B2547-9477-43A0-95D8-1B8F6E7085F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A26CDDAD-7B0D-427D-90B7-416B1D595C64}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A26CDDAD-7B0D-427D-90B7-416B1D595C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Resume" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>野口 慧</t>
   </si>
@@ -39,9 +39,6 @@
     <t>1984年7月10日生・男性</t>
   </si>
   <si>
-    <t>得意言語：GAS</t>
-  </si>
-  <si>
     <t>得意分野：アパレル・小売業界の自動化</t>
   </si>
   <si>
@@ -66,12 +63,6 @@
     <t>- 株式会社宮入・株式会社ファッションメッセージ：全国規模の仕入れルート開拓【2024年9月-2025年7月】業務企画・運営支援（11ヶ月）</t>
   </si>
   <si>
-    <t>- 倉庫未経験のアパレル工場に物流機能構築</t>
-  </si>
-  <si>
-    <t>- 物流業務代行体制設計・導入支援</t>
-  </si>
-  <si>
     <t>- 原価削減イベント企画・実行</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>- PL作成、代表への報告</t>
   </si>
   <si>
-    <t>【2018年12月-2020年3月】店舗管理・リテール営業（28ヶ月）株式会社東京白ゆり會</t>
-  </si>
-  <si>
     <t>- 店舗運営、売上管理</t>
   </si>
   <si>
@@ -120,40 +108,32 @@
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="ＭＳ ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>最寄駅：八王子</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>市丹木町1-144-12</t>
-    </r>
-    <rPh sb="7" eb="8">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="8" eb="11">
-      <t>タンギチョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
+    <t>最寄駅：八王子丹木町1-144-12</t>
+  </si>
+  <si>
+    <t>最終学歴：多摩大学 経済学部 卒業（2007年9月）</t>
+  </si>
+  <si>
+    <t>得意言語：GAS/Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  物流業務代行体制設計・導入支援</t>
+  </si>
+  <si>
+    <t>【2018年12月-2020年3月】全国店舗管理・リテール営業（28ヶ月）株式会社東京白ゆり會</t>
+  </si>
+  <si>
+    <t>【2018年11月まで】店長　店舗管理</t>
+  </si>
+  <si>
+    <t>"@ Set-Content -Path $path -Value $html -Encoding UTF8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,27 +187,6 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -257,15 +216,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -294,8 +247,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -322,69 +275,16 @@
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D124-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
 </file>
 
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D124-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D124-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1868809</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="photo" descr="写真">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6813239A-1CC8-EE24-ED0F-528F7D21FD6C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="45720" y="182880"/>
-          <a:ext cx="1478280" cy="1914529"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
@@ -408,7 +308,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C2E76EC-859F-E962-C48D-0D66FD71AE89}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -458,7 +358,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{472D19E8-8AAD-D01F-DA50-78C344A52B59}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -485,6 +385,1027 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="Text Box 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72312AD4-FC9A-D39F-DC37-38A731426CDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4968240"/>
+          <a:ext cx="762000" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="45720" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>印刷</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>Excel</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>写真選択</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>写真ここに画像をドラッグ</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>野口 慧</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>1984年7月10日生・男性</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>最寄駅：八王子丹木町1-144-12</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>最終学歴：多摩大学 経済学部 卒業（2007年9月）</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>得意言語：GAS/Python</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>得意分野：アパレル・小売業界の自動化</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>自己PR</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>全国17店舗を展開するアパレル事業において、過剰在庫と高原価構造による粗利圧迫を解消するため、仕組み設計から実装・全社展開まで一貫して推進しました。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>現場課題抽出、施策提案、代表との予算調整、プロトタイプ開発、運用定着まで実務で回し、短期で収益構造の改善を達成しています。</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>強み・アピール</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 商流改革力：独自の仕入れルートを開拓し原価構造を改善</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 技術実装力：GAS/Pythonでプロトタイプを自走し本番化</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 財務管理力：PL/BSを意識した予実管理・予算シミュレーション作成</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 推進力：現場・技術・経営を繋ぎ短期間で成果を出すPMO能力</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 少人数体制での全社改善再現力</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>職務経歴</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>直近フリーランス活動：</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 株式会社東京白ゆり会：物流設計・販売管理支援</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 株式会社アークリード：在庫処理・物流業務委託導入</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 株式会社宮入・株式会社ファッションメッセージ：全国規模の仕入れルート開拓【2024年9月-2025年7月】業務企画・運営支援（11ヶ月）</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>【2023年11月-2025年7月】個別プロジェクト対応（22ヶ月）フリーランス</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- ITツールによる業務効率化支援</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 経営企画支援　株式会社アークリード倉庫業務委託スキームPM</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 業務改善プロジェクト推進</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>  物流業務代行体制設計・導入支援</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 原価削減イベント企画・実行</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 商品管理・販売データ集計の自動化</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- クライアント折衝・関係者調整</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>【2020年4月-2023年9月】倉庫DX化PM　リテール営業担当（29ヶ月）株式会社東京白ゆり会（東京白ゆり會解散後M＆A）</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 店舗物流管理・フォーマット自動化</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- SATOとの連携・指示書作成　商品コントロール</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- PL作成、代表への報告</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>【2018年12月-2020年3月】全国店舗管理・リテール営業（28ヶ月）株式会社東京白ゆり會</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 店舗運営、売上管理</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 生産管理　商品コントロール</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>- 棚卸し・在庫管理</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>【2018年11月まで】店長　店舗管理</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="游ゴシック"/>
+            <a:ea typeface="游ゴシック"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="游ゴシック"/>
+              <a:ea typeface="游ゴシック"/>
+            </a:rPr>
+            <a:t>"@ Set-Content -Path $path -Value $html -Encoding UTF8</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>4198620</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>129540</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Control 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>2598420</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>830580</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Control 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1363980</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1995114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA5E97A8-FCE3-6B2A-B95E-FB78FE7644AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="243840"/>
+          <a:ext cx="1363980" cy="1979874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -786,10 +1707,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606DCC50-B12B-402A-8E1C-5852C6F94CE6}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -798,191 +1719,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:1" ht="158.4" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="4"/>
-    </row>
-    <row r="4" spans="1:1" ht="39.6">
-      <c r="A4" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="43.2">
-      <c r="A5" s="6" t="s">
+    <row r="4" spans="1:1" ht="21.6">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="6" spans="1:1" ht="37.799999999999997" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
+      <c r="A6" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="35.4" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="48" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:1" ht="60" customHeight="1">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="13" spans="1:1" ht="64.2" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="7"/>
+    </row>
+    <row r="15" spans="1:1" ht="87" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="8"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="35.4" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="48" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="33.6">
-      <c r="A10" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="7"/>
-    </row>
-    <row r="12" spans="1:1" ht="60" customHeight="1">
-      <c r="A12" s="9"/>
-    </row>
-    <row r="13" spans="1:1" ht="64.2" customHeight="1">
-      <c r="A13" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="9"/>
-    </row>
-    <row r="15" spans="1:1" ht="87" customHeight="1">
-      <c r="A15" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="10"/>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="10"/>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="11" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="11" t="s">
+    <row r="37" spans="1:1">
+      <c r="A37" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="11" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="10"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="11" t="s">
+    <row r="39" spans="1:1">
+      <c r="A39" s="8"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="8"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="8"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="3"/>
+    <row r="44" spans="1:1">
+      <c r="A44" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1040,6 +1971,56 @@
         <control shapeId="1026" r:id="rId5" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1030" r:id="rId7" name="Control 6">
+          <controlPr defaultSize="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>4198620</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>129540</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1030" r:id="rId7" name="Control 6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1031" r:id="rId9" name="Control 7">
+          <controlPr defaultSize="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>2598420</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>830580</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1031" r:id="rId9" name="Control 7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </controls>
 </worksheet>
 </file>
</xml_diff>